<commit_message>
fig: increase text size on timeline
</commit_message>
<xml_diff>
--- a/data_raw/ssmse_timeline.xlsx
+++ b/data_raw/ssmse_timeline.xlsx
@@ -48,13 +48,13 @@
     <t>Submit package to CRAN</t>
   </si>
   <si>
-    <t>More flexible estimation methods/ management procedures</t>
-  </si>
-  <si>
     <t>Automated plotting options</t>
   </si>
   <si>
     <t>More realistic sampling options</t>
+  </si>
+  <si>
+    <t>More flexible management procedures</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -405,7 +407,7 @@
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -419,7 +421,7 @@
         <v>2020</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -433,7 +435,7 @@
         <v>2020</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fix: rm duplicate item from timeline fig
</commit_message>
<xml_diff>
--- a/data_raw/ssmse_timeline.xlsx
+++ b/data_raw/ssmse_timeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>month</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>planned</t>
-  </si>
-  <si>
-    <t>Improve sampling from OMs</t>
   </si>
   <si>
     <t>Gather feedback from beta testers</t>
@@ -373,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +404,7 @@
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -421,7 +418,7 @@
         <v>2020</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -435,7 +432,7 @@
         <v>2020</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -443,7 +440,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -457,10 +454,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -471,7 +468,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>2021</v>
@@ -480,20 +477,6 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2021</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>